<commit_message>
finished 6, super cool btw
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Documents\DA_8\Projects\budget_lookups-pshanx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C537F2D-5E64-4619-9D45-7CA3BCC9246C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9D39F4-EC51-4181-9117-186A2EF946EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3830" yWindow="3320" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
   <si>
     <t>Department</t>
   </si>
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74:D79"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4283,11 +4283,11 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f>VLOOKUP(A56, A2:I52, 9, FALSE)</f>
+        <f>VLOOKUP($A56, $A2:Q52, 9, FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
-        <f>VLOOKUP(A56, A2:N52, 14, FALSE)</f>
+        <f>VLOOKUP($A56, $A2:R52, 14, FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4300,11 +4300,11 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:C61" si="10">VLOOKUP(A57, A3:I53, 9, FALSE)</f>
+        <f>VLOOKUP($A57, $A3:Q53, 9, FALSE)</f>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ref="D57:D61" si="11">VLOOKUP(A57, A3:N53, 14, FALSE)</f>
+        <f>VLOOKUP($A57, $A3:R53, 14, FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4317,11 +4317,11 @@
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="10"/>
+        <f>VLOOKUP($A58, $A4:Q54, 9, FALSE)</f>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="11"/>
+        <f>VLOOKUP($A58, $A4:R54, 14, FALSE)</f>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4334,11 +4334,11 @@
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="10"/>
+        <f>VLOOKUP($A59, $A5:Q55, 9, FALSE)</f>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="11"/>
+        <f>VLOOKUP($A59, $A5:R55, 14, FALSE)</f>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4351,11 +4351,11 @@
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="10"/>
+        <f>VLOOKUP($A60, $A6:Q56, 9, FALSE)</f>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="11"/>
+        <f>VLOOKUP($A60, $A6:R56, 14, FALSE)</f>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4368,11 +4368,11 @@
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="10"/>
+        <f>VLOOKUP($A61, $A7:Q57, 9, FALSE)</f>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="11"/>
+        <f>VLOOKUP($A61, $A7:R57, 14, FALSE)</f>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4400,11 +4400,11 @@
         <v>24</v>
       </c>
       <c r="B65">
-        <f>_xlfn.XLOOKUP(A65, A2:A52, D2:D52)</f>
+        <f>_xlfn.XLOOKUP($A65, $A2:$A52, D2:D52)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C65">
-        <f>_xlfn.XLOOKUP(A56, A2:A52, I2:I52)</f>
+        <f>_xlfn.XLOOKUP($A65, A2:A52, I2:I52)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D65">
@@ -4417,15 +4417,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP(A66, A3:A53, D3:D53)</f>
+        <f t="shared" ref="B66:C70" si="10">_xlfn.XLOOKUP($A66, A3:A53, D3:D53)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP(A57, A3:A53, I3:I53)</f>
+        <f t="shared" ref="C66:C70" si="11">_xlfn.XLOOKUP($A66, A3:A53, I3:I53)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP(A57, A3:A53, N3:N53)</f>
+        <f t="shared" ref="D66:D70" si="12">_xlfn.XLOOKUP(A57, A3:A53, N3:N53)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4434,15 +4434,15 @@
         <v>32</v>
       </c>
       <c r="B67">
+        <f t="shared" si="10"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="11"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D67">
         <f t="shared" si="12"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="C67">
-        <f t="shared" si="13"/>
-        <v>-189254.06000000006</v>
-      </c>
-      <c r="D67">
-        <f t="shared" si="14"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4451,15 +4451,15 @@
         <v>38</v>
       </c>
       <c r="B68">
+        <f t="shared" si="10"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="11"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D68">
         <f t="shared" si="12"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="C68">
-        <f t="shared" si="13"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="D68">
-        <f t="shared" si="14"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4468,15 +4468,15 @@
         <v>39</v>
       </c>
       <c r="B69">
+        <f t="shared" si="10"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="11"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D69">
         <f t="shared" si="12"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="C69">
-        <f t="shared" si="13"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="D69">
-        <f t="shared" si="14"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4485,15 +4485,15 @@
         <v>55</v>
       </c>
       <c r="B70">
+        <f t="shared" si="10"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="11"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D70">
         <f t="shared" si="12"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="C70">
-        <f t="shared" si="13"/>
-        <v>-133456.33000001032</v>
-      </c>
-      <c r="D70">
-        <f t="shared" si="14"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4538,15 +4538,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="15">INDEX(D3:D53, MATCH(A75, A3:A53, 0))</f>
+        <f t="shared" ref="B75:B79" si="13">INDEX(D3:D53, MATCH(A75, A3:A53, 0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="16">INDEX(I3:I53, MATCH(A75, A3:A53))</f>
+        <f t="shared" ref="C75:C79" si="14">INDEX(I3:I53, MATCH(A75, A3:A53))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="17">INDEX(N3:N53, MATCH(A75, A3:A53))</f>
+        <f t="shared" ref="D75:D79" si="15">INDEX(N3:N53, MATCH(A75, A3:A53))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4555,15 +4555,15 @@
         <v>32</v>
       </c>
       <c r="B76">
+        <f t="shared" si="13"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="14"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D76">
         <f t="shared" si="15"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="C76">
-        <f t="shared" si="16"/>
-        <v>-189254.06000000006</v>
-      </c>
-      <c r="D76">
-        <f t="shared" si="17"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4572,15 +4572,15 @@
         <v>38</v>
       </c>
       <c r="B77">
+        <f t="shared" si="13"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="14"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D77">
         <f t="shared" si="15"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="C77">
-        <f t="shared" si="16"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="D77">
-        <f t="shared" si="17"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4589,15 +4589,15 @@
         <v>39</v>
       </c>
       <c r="B78">
+        <f t="shared" si="13"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="14"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
         <f t="shared" si="15"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="C78">
-        <f t="shared" si="16"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="D78">
-        <f t="shared" si="17"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4606,15 +4606,15 @@
         <v>55</v>
       </c>
       <c r="B79">
+        <f t="shared" si="13"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="14"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
         <f t="shared" si="15"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="C79">
-        <f t="shared" si="16"/>
-        <v>-133456.33000001032</v>
-      </c>
-      <c r="D79">
-        <f t="shared" si="17"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4627,6 +4627,9 @@
       <c r="A82" t="s">
         <v>0</v>
       </c>
+      <c r="B82" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B83" s="1" t="s">
@@ -4640,22 +4643,40 @@
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
+      <c r="B84" s="6">
+        <f>INDEX(B2:B52,MATCH(B82,A2:A52,0))</f>
+        <v>356640100</v>
+      </c>
+      <c r="C84" s="6">
+        <f>INDEX(C2:C52,MATCH(B82,A2:A52))</f>
+        <v>341243679.13</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
+      <c r="B85" s="6">
+        <f>INDEX(G2:G52,MATCH(B82,A2:A52,0))</f>
+        <v>382685200</v>
+      </c>
+      <c r="C85" s="6">
+        <f>INDEX(H2:H52,MATCH(B82,A2:A52,0))</f>
+        <v>346340810.81999999</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
+      <c r="B86" s="6">
+        <f>INDEX(L2:L52,MATCH(B82,A2:A52,0))</f>
+        <v>376548600</v>
+      </c>
+      <c r="C86" s="6">
+        <f>INDEX(M2:M52,MATCH(B82,A2:A52,0))</f>
+        <v>355279492.22999901</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="7" t="s">
@@ -4791,11 +4812,14 @@
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82" xr:uid="{E7A19135-B653-4F1F-9DBF-0D9049A208D4}">
+      <formula1>$A$2:$A$52</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished 7, sort of
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Documents\DA_8\Projects\budget_lookups-pshanx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9D39F4-EC51-4181-9117-186A2EF946EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F424AEF-4BC3-4F68-A332-1FD088EE088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,6 +31,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1178,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4279,7 +4301,7 @@
         <v>24</v>
       </c>
       <c r="B56">
-        <f>VLOOKUP(A56, A2:D52, 4, FALSE)</f>
+        <f>VLOOKUP($A56,$A$1:$P$52,MATCH(B$55,$A$1:$P$1,FALSE))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
@@ -4296,7 +4318,7 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="9">VLOOKUP(A57, A3:D53, 4, FALSE)</f>
+        <f t="shared" ref="B57:D61" si="9">VLOOKUP($A57,$A$1:$P$52,MATCH(B$55,$A$1:$P$1,FALSE))</f>
         <v>0</v>
       </c>
       <c r="C57">
@@ -4399,16 +4421,16 @@
       <c r="A65" t="s">
         <v>24</v>
       </c>
-      <c r="B65">
-        <f>_xlfn.XLOOKUP($A65, $A2:$A52, D2:D52)</f>
+      <c r="B65" cm="1">
+        <f t="array" ref="B65">_xlfn.XLOOKUP($A65, $A$2:$A$52, _xlfn.XLOOKUP(B$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-36209.630000000005</v>
       </c>
-      <c r="C65">
-        <f>_xlfn.XLOOKUP($A65, A2:A52, I2:I52)</f>
+      <c r="C65" cm="1">
+        <f t="array" ref="C65">_xlfn.XLOOKUP($A65, $A$2:$A$52, _xlfn.XLOOKUP(C$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-27292.159999999974</v>
       </c>
-      <c r="D65">
-        <f>_xlfn.XLOOKUP(A56, A2:A52, N2:N52)</f>
+      <c r="D65" cm="1">
+        <f t="array" ref="D65">_xlfn.XLOOKUP($A65, $A$2:$A$52, _xlfn.XLOOKUP(D$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4416,16 +4438,16 @@
       <c r="A66" t="s">
         <v>25</v>
       </c>
-      <c r="B66">
-        <f t="shared" ref="B66:C70" si="10">_xlfn.XLOOKUP($A66, A3:A53, D3:D53)</f>
-        <v>0</v>
-      </c>
-      <c r="C66">
-        <f t="shared" ref="C66:C70" si="11">_xlfn.XLOOKUP($A66, A3:A53, I3:I53)</f>
-        <v>0</v>
-      </c>
-      <c r="D66">
-        <f t="shared" ref="D66:D70" si="12">_xlfn.XLOOKUP(A57, A3:A53, N3:N53)</f>
+      <c r="B66" cm="1">
+        <f t="array" ref="B66">_xlfn.XLOOKUP($A66, $A$2:$A$52, _xlfn.XLOOKUP(B$64, $A$1:$P$1,$A$2:$P$52))</f>
+        <v>0</v>
+      </c>
+      <c r="C66" cm="1">
+        <f t="array" ref="C66">_xlfn.XLOOKUP($A66, $A$2:$A$52, _xlfn.XLOOKUP(C$64, $A$1:$P$1,$A$2:$P$52))</f>
+        <v>0</v>
+      </c>
+      <c r="D66" cm="1">
+        <f t="array" ref="D66">_xlfn.XLOOKUP($A66, $A$2:$A$52, _xlfn.XLOOKUP(D$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4433,16 +4455,16 @@
       <c r="A67" t="s">
         <v>32</v>
       </c>
-      <c r="B67">
-        <f t="shared" si="10"/>
+      <c r="B67" cm="1">
+        <f t="array" ref="B67">_xlfn.XLOOKUP($A67, $A$2:$A$52, _xlfn.XLOOKUP(B$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-149396.10000000987</v>
       </c>
-      <c r="C67">
-        <f t="shared" si="11"/>
+      <c r="C67" cm="1">
+        <f t="array" ref="C67">_xlfn.XLOOKUP($A67, $A$2:$A$52, _xlfn.XLOOKUP(C$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-189254.06000000006</v>
       </c>
-      <c r="D67">
-        <f t="shared" si="12"/>
+      <c r="D67" cm="1">
+        <f t="array" ref="D67">_xlfn.XLOOKUP($A67, $A$2:$A$52, _xlfn.XLOOKUP(D$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4450,16 +4472,16 @@
       <c r="A68" t="s">
         <v>38</v>
       </c>
-      <c r="B68">
-        <f t="shared" si="10"/>
+      <c r="B68" cm="1">
+        <f t="array" ref="B68">_xlfn.XLOOKUP($A68, $A$2:$A$52, _xlfn.XLOOKUP(B$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-12230.810000000056</v>
       </c>
-      <c r="C68">
-        <f t="shared" si="11"/>
+      <c r="C68" cm="1">
+        <f t="array" ref="C68">_xlfn.XLOOKUP($A68, $A$2:$A$52, _xlfn.XLOOKUP(C$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-45485.580000000075</v>
       </c>
-      <c r="D68">
-        <f t="shared" si="12"/>
+      <c r="D68" cm="1">
+        <f t="array" ref="D68">_xlfn.XLOOKUP($A68, $A$2:$A$52, _xlfn.XLOOKUP(D$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4467,16 +4489,16 @@
       <c r="A69" t="s">
         <v>39</v>
       </c>
-      <c r="B69">
-        <f t="shared" si="10"/>
+      <c r="B69" cm="1">
+        <f t="array" ref="B69">_xlfn.XLOOKUP($A69, $A$2:$A$52, _xlfn.XLOOKUP(B$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="C69">
-        <f t="shared" si="11"/>
+      <c r="C69" cm="1">
+        <f t="array" ref="C69">_xlfn.XLOOKUP($A69, $A$2:$A$52, _xlfn.XLOOKUP(C$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="D69">
-        <f t="shared" si="12"/>
+      <c r="D69" cm="1">
+        <f t="array" ref="D69">_xlfn.XLOOKUP($A69, $A$2:$A$52, _xlfn.XLOOKUP(D$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4484,16 +4506,16 @@
       <c r="A70" t="s">
         <v>55</v>
       </c>
-      <c r="B70">
-        <f t="shared" si="10"/>
+      <c r="B70" cm="1">
+        <f t="array" ref="B70">_xlfn.XLOOKUP($A70, $A$2:$A$52, _xlfn.XLOOKUP(B$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C70">
-        <f t="shared" si="11"/>
+      <c r="C70" cm="1">
+        <f t="array" ref="C70">_xlfn.XLOOKUP($A70, $A$2:$A$52, _xlfn.XLOOKUP(C$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D70">
-        <f t="shared" si="12"/>
+      <c r="D70" cm="1">
+        <f t="array" ref="D70">_xlfn.XLOOKUP($A70, $A$2:$A$52, _xlfn.XLOOKUP(D$64, $A$1:$P$1,$A$2:$P$52))</f>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4521,15 +4543,15 @@
         <v>24</v>
       </c>
       <c r="B74">
-        <f>INDEX(D2:D52, MATCH(A74, A2:A52, 0))</f>
+        <f>INDEX($A$2:$P$52,MATCH($A74,$A$2:$A$52,0),MATCH(B$73,$A$1:$P$1,0))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C74">
-        <f>INDEX(I2:I52, MATCH(A74, A2:A52))</f>
+        <f t="shared" ref="C74:D74" si="10">INDEX($A$2:$P$52,MATCH($A74,$A$2:$A$52,0),MATCH(C$73,$A$1:$P$1,0))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D74">
-        <f>INDEX(N2:N52, MATCH(A74, A2:A52))</f>
+        <f t="shared" si="10"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4538,15 +4560,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="13">INDEX(D3:D53, MATCH(A75, A3:A53, 0))</f>
+        <f t="shared" ref="B75:D79" si="11">INDEX($A$2:$P$52,MATCH($A75,$A$2:$A$52,0),MATCH(B$73,$A$1:$P$1,0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="14">INDEX(I3:I53, MATCH(A75, A3:A53))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="15">INDEX(N3:N53, MATCH(A75, A3:A53))</f>
+        <f t="shared" si="11"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4555,15 +4577,15 @@
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4572,15 +4594,15 @@
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4589,15 +4611,15 @@
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4606,15 +4628,15 @@
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4723,24 +4745,57 @@
       <c r="A91" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="5"/>
+      <c r="B91" t="str">
+        <f>_xlfn.XLOOKUP($B$89, F2:F52, $A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="D91" s="5" t="str">
+        <f>_xlfn.XLOOKUP($D$89, F2:F52, $A$2:$A$52)</f>
+        <v>Circuit Court Clerk</v>
+      </c>
       <c r="E91" s="5"/>
+      <c r="F91" t="str">
+        <f>_xlfn.XLOOKUP($F$89, F2:F52, $A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
       <c r="G91" s="5"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
+      <c r="B92" t="str">
+        <f>_xlfn.XLOOKUP($B$89, K2:K52, $A$2:$A$52)</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="D92" s="5" t="str">
+        <f>_xlfn.XLOOKUP($D$89,K2:K52, $A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
       <c r="E92" s="5"/>
+      <c r="F92" t="str">
+        <f>_xlfn.XLOOKUP($F$89, K2:K52, $A$2:$A$52)</f>
+        <v>Office of Family Safety</v>
+      </c>
       <c r="G92" s="5"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
+      <c r="B93" t="str">
+        <f>_xlfn.XLOOKUP($B$89, P2:P52, $A$2:$A$52)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="D93" s="5" t="str">
+        <f>_xlfn.XLOOKUP($D$89, P2:P52, $A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
       <c r="E93" s="5"/>
+      <c r="F93" t="str">
+        <f>_xlfn.XLOOKUP($F$89, P2:P52, $A$2:$A$52)</f>
+        <v>Election Commission</v>
+      </c>
       <c r="G93" s="5"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
@@ -4812,14 +4867,11 @@
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 B82" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82" xr:uid="{E7A19135-B653-4F1F-9DBF-0D9049A208D4}">
-      <formula1>$A$2:$A$52</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished 9, going back for the bonuses
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Documents\DA_8\Projects\budget_lookups-pshanx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F424AEF-4BC3-4F68-A332-1FD088EE088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72225BB0-0D08-4096-8D96-12068915F26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1200,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4318,7 +4318,7 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:D61" si="9">VLOOKUP($A57,$A$1:$P$52,MATCH(B$55,$A$1:$P$1,FALSE))</f>
+        <f t="shared" ref="B57:B61" si="9">VLOOKUP($A57,$A$1:$P$52,MATCH(B$55,$A$1:$P$1,FALSE))</f>
         <v>0</v>
       </c>
       <c r="C57">
@@ -4746,57 +4746,87 @@
         <v>73</v>
       </c>
       <c r="B91" t="str">
-        <f>_xlfn.XLOOKUP($B$89, F2:F52, $A$2:$A$52)</f>
+        <f>_xlfn.XLOOKUP(B$89, $F$2:$F$52, $A$2:$A$52)</f>
         <v>Clerk and Master - Chancery</v>
       </c>
-      <c r="D91" s="5" t="str">
-        <f>_xlfn.XLOOKUP($D$89, F2:F52, $A$2:$A$52)</f>
+      <c r="C91" s="5">
+        <f>_xlfn.XLOOKUP(B$91, $A$2:$A$52,$E$2:$E$52)</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" ref="C91:G91" si="12">_xlfn.XLOOKUP(D$89, $F$2:$F$52, $A$2:$A$52)</f>
         <v>Circuit Court Clerk</v>
       </c>
-      <c r="E91" s="5"/>
+      <c r="E91" s="5">
+        <f>_xlfn.XLOOKUP(D$91, $A$2:$A$52,$E$2:$E$52)</f>
+        <v>-0.11502817362571344</v>
+      </c>
       <c r="F91" t="str">
-        <f>_xlfn.XLOOKUP($F$89, F2:F52, $A$2:$A$52)</f>
+        <f t="shared" si="12"/>
         <v>Internal Audit</v>
       </c>
-      <c r="G91" s="5"/>
+      <c r="G91" s="5">
+        <f>_xlfn.XLOOKUP(F$91, $A$2:$A$52,$E$2:$E$52)</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>74</v>
       </c>
       <c r="B92" t="str">
-        <f>_xlfn.XLOOKUP($B$89, K2:K52, $A$2:$A$52)</f>
+        <f>_xlfn.XLOOKUP(B$89, $K$2:$K$52, $A$2:$A$52)</f>
         <v>Metropolitan Clerk</v>
       </c>
-      <c r="D92" s="5" t="str">
-        <f>_xlfn.XLOOKUP($D$89,K2:K52, $A$2:$A$52)</f>
+      <c r="C92" s="5">
+        <f>_xlfn.XLOOKUP(B$92, $A$2:$A$52,$J$2:$J$52)</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D92" t="str">
+        <f>_xlfn.XLOOKUP(D$89, $K$2:$K$52, $A$2:$A$52)</f>
         <v>Internal Audit</v>
       </c>
-      <c r="E92" s="5"/>
+      <c r="E92" s="5">
+        <f>_xlfn.XLOOKUP(D$92, $A$2:$A$52,$J$2:$J$52)</f>
+        <v>-0.17103239309050916</v>
+      </c>
       <c r="F92" t="str">
-        <f>_xlfn.XLOOKUP($F$89, K2:K52, $A$2:$A$52)</f>
+        <f>_xlfn.XLOOKUP(F$89, $K$2:$K$52, $A$2:$A$52)</f>
         <v>Office of Family Safety</v>
       </c>
-      <c r="G92" s="5"/>
+      <c r="G92" s="5">
+        <f>_xlfn.XLOOKUP(F$92, $A$2:$A$52,$J$2:$J$52)</f>
+        <v>-0.13918241656366656</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>75</v>
       </c>
       <c r="B93" t="str">
-        <f>_xlfn.XLOOKUP($B$89, P2:P52, $A$2:$A$52)</f>
+        <f>_xlfn.XLOOKUP(B$89, $P$2:$P$52, $A$2:$A$52)</f>
         <v>Community Oversight Board</v>
       </c>
-      <c r="D93" s="5" t="str">
-        <f>_xlfn.XLOOKUP($D$89, P2:P52, $A$2:$A$52)</f>
+      <c r="C93" s="5">
+        <f>_xlfn.XLOOKUP(B$93,$A$2:$A$52,$O$2:$O$52)</f>
+        <v>-4.8803319517950765</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" ref="C93:G93" si="13">_xlfn.XLOOKUP(D$89, $P$2:$P$52, $A$2:$A$52)</f>
         <v>Clerk and Master - Chancery</v>
       </c>
-      <c r="E93" s="5"/>
+      <c r="E93" s="5">
+        <f>_xlfn.XLOOKUP(D$93,$A$2:$A$52,$O$2:$O$52)</f>
+        <v>-0.18057733573186341</v>
+      </c>
       <c r="F93" t="str">
-        <f>_xlfn.XLOOKUP($F$89, P2:P52, $A$2:$A$52)</f>
+        <f t="shared" si="13"/>
         <v>Election Commission</v>
       </c>
-      <c r="G93" s="5"/>
+      <c r="G93" s="5">
+        <f>_xlfn.XLOOKUP(F$93,$A$2:$A$52,$O$2:$O$52)</f>
+        <v>-0.14787719878320607</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
@@ -4843,27 +4873,90 @@
       <c r="A98" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="G98" s="4"/>
+      <c r="B98" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(B$96,$F$2:$F$52, 0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C98" s="5">
+        <f>INDEX($E$2:$E$52,MATCH(B$96,$F$2:$F$52,0))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D98" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(D$96,$F$2:$F$52, 0))</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E98" s="5">
+        <f>INDEX($E$2:$E$52, MATCH(D$98, $A$2:$A$52))</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F98" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(F$96,$F$2:$F$52, 0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G98" s="5">
+        <f>INDEX($E$2:$E$52, MATCH(F$98, $A$2:$A$52))</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="G99" s="4"/>
+      <c r="B99" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(B$96,$K$2:$K$52, 0))</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C99" s="5">
+        <f>INDEX($J$2:$J$52, MATCH(B$99, $A$2:$A$52,0))</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D99" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(D$96,$K$2:$K$52, 0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E99" s="5">
+        <f>INDEX($J$2:$J$52, MATCH(D$99, $A$2:$A$52,0))</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F99" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(F$96,$K$2:$K$52, 0))</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G99" s="5">
+        <f>INDEX($J$2:$J$52, MATCH(F$99, $A$2:$A$52,0))</f>
+        <v>-0.13918241656366656</v>
+      </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>75</v>
       </c>
-      <c r="C100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="G100" s="4"/>
+      <c r="B100" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(B$96,$P$2:$P$52,0))</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C100" s="5">
+        <f>INDEX($O$2:$O$52, MATCH(B$100, $A$2:$A$52,0))</f>
+        <v>-4.8803319517950765</v>
+      </c>
+      <c r="D100" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(D$96,$P$2:$P$52,0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E100" s="5">
+        <f>INDEX($O$2:$O$52, MATCH(D$100, $A$2:$A$52,0))</f>
+        <v>-0.18057733573186341</v>
+      </c>
+      <c r="F100" t="str">
+        <f>INDEX($A$2:$A$52,MATCH(F$96,$P$2:$P$52,0))</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G100" s="5">
+        <f>INDEX($O$2:$O$52, MATCH(F$100, $A$2:$A$52,0))</f>
+        <v>-0.14787719878320607</v>
+      </c>
       <c r="I100" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
these bonuses are making me crazy
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Documents\DA_8\Projects\budget_lookups-pshanx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72225BB0-0D08-4096-8D96-12068915F26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9FEA47-5E0B-4CF2-A8A4-F6E2FF887FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="92">
   <si>
     <t>Department</t>
   </si>
@@ -326,14 +326,19 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>What the fuck?</t>
+  </si>
+  <si>
+    <t>XLOOKUP("","", A2:A52)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
@@ -836,13 +841,13 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1200,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1282,7 +1287,7 @@
         <f>C2-B2</f>
         <v>-15396420.870000005</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <f>IFERROR((C2-B2)/B2, 0)</f>
         <v>-4.3170750765267295E-2</v>
       </c>
@@ -1300,7 +1305,7 @@
         <f>H2-G2</f>
         <v>-36344389.180000007</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <f>IFERROR((H2-G2)/G2, 0)</f>
         <v>-9.4972027086493035E-2</v>
       </c>
@@ -1318,7 +1323,7 @@
         <f>M2-L2</f>
         <v>-21269107.770000994</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="4">
         <f>IFERROR((M2-L2)/M2, 0)</f>
         <v>-5.9865847129256501E-2</v>
       </c>
@@ -1341,7 +1346,7 @@
         <f t="shared" ref="D3:D52" si="0">C3-B3</f>
         <v>-7585.4099999999744</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <f t="shared" ref="E3:E52" si="1">IFERROR((C3-B3)/B3, 0)</f>
         <v>-2.3069981751824741E-2</v>
       </c>
@@ -1359,7 +1364,7 @@
         <f t="shared" ref="I3:I52" si="3">H3-G3</f>
         <v>-22366.290000001027</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <f t="shared" ref="J3:J52" si="4">IFERROR((H3-G3)/G3, 0)</f>
         <v>-6.6804928315415249E-2</v>
       </c>
@@ -1377,7 +1382,7 @@
         <f t="shared" ref="N3:N52" si="6">M3-L3</f>
         <v>-436.96000000002095</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="4">
         <f t="shared" ref="O3:O52" si="7">IFERROR((M3-L3)/M3, 0)</f>
         <v>-1.3559109974262671E-3</v>
       </c>
@@ -1400,7 +1405,7 @@
         <f t="shared" si="0"/>
         <v>-15442.440000010189</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <f t="shared" si="1"/>
         <v>-4.9327413275443007E-3</v>
       </c>
@@ -1418,7 +1423,7 @@
         <f t="shared" si="3"/>
         <v>-62606.790000009816</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <f t="shared" si="4"/>
         <v>-1.7141743558856015E-2</v>
       </c>
@@ -1436,7 +1441,7 @@
         <f t="shared" si="6"/>
         <v>-97416.950000009965</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="4">
         <f t="shared" si="7"/>
         <v>-2.7326062602179901E-2</v>
       </c>
@@ -1459,7 +1464,7 @@
         <f t="shared" si="0"/>
         <v>-723147.33000000007</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <f t="shared" si="1"/>
         <v>-9.4273968477453174E-2</v>
       </c>
@@ -1477,7 +1482,7 @@
         <f t="shared" si="3"/>
         <v>-947690.6799999997</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <f t="shared" si="4"/>
         <v>-0.118932605449092</v>
       </c>
@@ -1495,7 +1500,7 @@
         <f t="shared" si="6"/>
         <v>-262277.08999999985</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="4">
         <f t="shared" si="7"/>
         <v>-3.4982765601595231E-2</v>
       </c>
@@ -1518,7 +1523,7 @@
         <f t="shared" si="0"/>
         <v>-23391.479999999981</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <f t="shared" si="1"/>
         <v>-5.7149963352064452E-2</v>
       </c>
@@ -1536,7 +1541,7 @@
         <f t="shared" si="3"/>
         <v>-741.35999999998603</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <f t="shared" si="4"/>
         <v>-1.7301283547257551E-3</v>
       </c>
@@ -1554,7 +1559,7 @@
         <f t="shared" si="6"/>
         <v>-85.710000001010485</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="4">
         <f t="shared" si="7"/>
         <v>-1.9255728680607105E-4</v>
       </c>
@@ -1577,7 +1582,7 @@
         <f t="shared" si="0"/>
         <v>-382928.79000000004</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f t="shared" si="1"/>
         <v>-0.11502817362571344</v>
       </c>
@@ -1595,7 +1600,7 @@
         <f t="shared" si="3"/>
         <v>-339416.58999999985</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <f t="shared" si="4"/>
         <v>-0.10009631366303927</v>
       </c>
@@ -1613,7 +1618,7 @@
         <f t="shared" si="6"/>
         <v>-398759.91999999993</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="4">
         <f t="shared" si="7"/>
         <v>-0.13533617150632837</v>
       </c>
@@ -1636,7 +1641,7 @@
         <f t="shared" si="0"/>
         <v>-236476.69000000996</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f t="shared" si="1"/>
         <v>-0.15235918433091292</v>
       </c>
@@ -1654,7 +1659,7 @@
         <f t="shared" si="3"/>
         <v>-206794.01000001002</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <f t="shared" si="4"/>
         <v>-0.13000189224870184</v>
       </c>
@@ -1672,7 +1677,7 @@
         <f t="shared" si="6"/>
         <v>-241564.68000000995</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="4">
         <f t="shared" si="7"/>
         <v>-0.18057733573186341</v>
       </c>
@@ -1695,7 +1700,7 @@
         <f t="shared" si="0"/>
         <v>-396574.72000000067</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <f t="shared" si="1"/>
         <v>-4.2417130511048909E-2</v>
       </c>
@@ -1713,7 +1718,7 @@
         <f t="shared" si="3"/>
         <v>-1144640.4800000004</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <f t="shared" si="4"/>
         <v>-0.10336567542917005</v>
       </c>
@@ -1731,7 +1736,7 @@
         <f t="shared" si="6"/>
         <v>-796900.47000000998</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="4">
         <f t="shared" si="7"/>
         <v>-7.9741085042259116E-2</v>
       </c>
@@ -1754,7 +1759,7 @@
         <f t="shared" si="0"/>
         <v>-36209.630000000005</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f t="shared" si="1"/>
         <v>-8.1681998646514792E-2</v>
       </c>
@@ -1772,7 +1777,7 @@
         <f t="shared" si="3"/>
         <v>-27292.159999999974</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <f t="shared" si="4"/>
         <v>-5.5113408723747932E-2</v>
       </c>
@@ -1790,7 +1795,7 @@
         <f t="shared" si="6"/>
         <v>-9181.0800000000163</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="4">
         <f t="shared" si="7"/>
         <v>-1.9194473846027283E-2</v>
       </c>
@@ -1813,7 +1818,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1831,7 +1836,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1849,7 +1854,7 @@
         <f t="shared" si="6"/>
         <v>-311228.08999999997</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="4">
         <f t="shared" si="7"/>
         <v>-4.8803319517950765</v>
       </c>
@@ -1872,7 +1877,7 @@
         <f t="shared" si="0"/>
         <v>-214304.66999999993</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <f t="shared" si="1"/>
         <v>-5.0060657805601608E-2</v>
       </c>
@@ -1890,7 +1895,7 @@
         <f t="shared" si="3"/>
         <v>-494844.40000000037</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="4">
         <f t="shared" si="4"/>
         <v>-0.10527708280146378</v>
       </c>
@@ -1908,7 +1913,7 @@
         <f t="shared" si="6"/>
         <v>-306086.86000000034</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="4">
         <f t="shared" si="7"/>
         <v>-7.0015312120868103E-2</v>
       </c>
@@ -1931,7 +1936,7 @@
         <f t="shared" si="0"/>
         <v>-75511.669999999925</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f t="shared" si="1"/>
         <v>-1.2912833886247806E-2</v>
       </c>
@@ -1949,7 +1954,7 @@
         <f t="shared" si="3"/>
         <v>-314622.06000000983</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <f t="shared" si="4"/>
         <v>-5.0552253482656594E-2</v>
       </c>
@@ -1967,7 +1972,7 @@
         <f t="shared" si="6"/>
         <v>-150323.33000000007</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="4">
         <f t="shared" si="7"/>
         <v>-2.4818211822499901E-2</v>
       </c>
@@ -1990,7 +1995,7 @@
         <f t="shared" si="0"/>
         <v>-6982.6300000000047</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <f t="shared" si="1"/>
         <v>-1.3637949218750009E-2</v>
       </c>
@@ -2008,7 +2013,7 @@
         <f t="shared" si="3"/>
         <v>-6097.0200000000186</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="4">
         <f t="shared" si="4"/>
         <v>-1.1492968897266765E-2</v>
       </c>
@@ -2026,7 +2031,7 @@
         <f t="shared" si="6"/>
         <v>-21210.119999999995</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="4">
         <f t="shared" si="7"/>
         <v>-4.200107930875762E-2</v>
       </c>
@@ -2049,7 +2054,7 @@
         <f t="shared" si="0"/>
         <v>496819.90000000596</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <f t="shared" si="1"/>
         <v>3.1837408866824991E-3</v>
       </c>
@@ -2067,7 +2072,7 @@
         <f t="shared" si="3"/>
         <v>-8201410.7500010133</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="4">
         <f t="shared" si="4"/>
         <v>-4.4532273014072019E-2</v>
       </c>
@@ -2085,7 +2090,7 @@
         <f t="shared" si="6"/>
         <v>-4502589.1500009894</v>
       </c>
-      <c r="O15" s="5">
+      <c r="O15" s="4">
         <f t="shared" si="7"/>
         <v>-2.4410772108697416E-2</v>
       </c>
@@ -2108,7 +2113,7 @@
         <f t="shared" si="0"/>
         <v>-78219.540000010282</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>-1.1850188616360429E-2</v>
       </c>
@@ -2126,7 +2131,7 @@
         <f t="shared" si="3"/>
         <v>-2035.9199999999255</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="4">
         <f t="shared" si="4"/>
         <v>-2.769017341040361E-4</v>
       </c>
@@ -2144,7 +2149,7 @@
         <f t="shared" si="6"/>
         <v>-107</v>
       </c>
-      <c r="O16" s="5">
+      <c r="O16" s="4">
         <f t="shared" si="7"/>
         <v>-1.4465141914533183E-5</v>
       </c>
@@ -2167,7 +2172,7 @@
         <f t="shared" si="0"/>
         <v>-421319.94999999925</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <f t="shared" si="1"/>
         <v>-2.8351094826658003E-2</v>
       </c>
@@ -2185,7 +2190,7 @@
         <f t="shared" si="3"/>
         <v>-664466.49000000022</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="4">
         <f t="shared" si="4"/>
         <v>-4.3401666263871937E-2</v>
       </c>
@@ -2203,7 +2208,7 @@
         <f t="shared" si="6"/>
         <v>-965742.96000000089</v>
       </c>
-      <c r="O17" s="5">
+      <c r="O17" s="4">
         <f t="shared" si="7"/>
         <v>-6.7317657897727201E-2</v>
       </c>
@@ -2226,7 +2231,7 @@
         <f t="shared" si="0"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <f t="shared" si="1"/>
         <v>-5.4037002206391245E-2</v>
       </c>
@@ -2244,7 +2249,7 @@
         <f t="shared" si="3"/>
         <v>-189254.06000000006</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="4">
         <f t="shared" si="4"/>
         <v>-6.6149619014330668E-2</v>
       </c>
@@ -2262,7 +2267,7 @@
         <f t="shared" si="6"/>
         <v>-374962.91000000015</v>
       </c>
-      <c r="O18" s="5">
+      <c r="O18" s="4">
         <f t="shared" si="7"/>
         <v>-0.14787719878320607</v>
       </c>
@@ -2285,7 +2290,7 @@
         <f t="shared" si="0"/>
         <v>-376336.80000001006</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <f t="shared" si="1"/>
         <v>-4.258504294298146E-2</v>
       </c>
@@ -2303,7 +2308,7 @@
         <f t="shared" si="3"/>
         <v>-721592.76000000909</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="4">
         <f t="shared" si="4"/>
         <v>-7.4289145810384635E-2</v>
       </c>
@@ -2321,7 +2326,7 @@
         <f t="shared" si="6"/>
         <v>-576344.08999999985</v>
       </c>
-      <c r="O19" s="5">
+      <c r="O19" s="4">
         <f t="shared" si="7"/>
         <v>-6.5742752529225235E-2</v>
       </c>
@@ -2344,7 +2349,7 @@
         <f t="shared" si="0"/>
         <v>-1539.8400010019541</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <f t="shared" si="1"/>
         <v>-1.2379538203300809E-5</v>
       </c>
@@ -2362,7 +2367,7 @@
         <f t="shared" si="3"/>
         <v>-9775.6299999952316</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="4">
         <f t="shared" si="4"/>
         <v>-7.4142392760188761E-5</v>
       </c>
@@ -2380,7 +2385,7 @@
         <f t="shared" si="6"/>
         <v>-116.46000100672245</v>
       </c>
-      <c r="O20" s="5">
+      <c r="O20" s="4">
         <f t="shared" si="7"/>
         <v>-8.9158518313793741E-7</v>
       </c>
@@ -2403,7 +2408,7 @@
         <f t="shared" si="0"/>
         <v>-1923512.4500000998</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <f t="shared" si="1"/>
         <v>-7.9052463618023094E-2</v>
       </c>
@@ -2421,7 +2426,7 @@
         <f t="shared" si="3"/>
         <v>-1841406.370000001</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="4">
         <f t="shared" si="4"/>
         <v>-7.5167420624229556E-2</v>
       </c>
@@ -2439,7 +2444,7 @@
         <f t="shared" si="6"/>
         <v>-888926.91000010073</v>
       </c>
-      <c r="O21" s="5">
+      <c r="O21" s="4">
         <f t="shared" si="7"/>
         <v>-3.793309454084768E-2</v>
       </c>
@@ -2462,7 +2467,7 @@
         <f t="shared" si="0"/>
         <v>-153660.12000009976</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <f t="shared" si="1"/>
         <v>-1.3285502334437123E-2</v>
       </c>
@@ -2480,7 +2485,7 @@
         <f t="shared" si="3"/>
         <v>-188722.03000009991</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22" s="4">
         <f t="shared" si="4"/>
         <v>-1.5752170574348738E-2</v>
       </c>
@@ -2498,7 +2503,7 @@
         <f t="shared" si="6"/>
         <v>-745.23000000044703</v>
       </c>
-      <c r="O22" s="5">
+      <c r="O22" s="4">
         <f t="shared" si="7"/>
         <v>-6.2443573197307203E-5</v>
       </c>
@@ -2521,7 +2526,7 @@
         <f t="shared" si="0"/>
         <v>-825956.59000010043</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <f t="shared" si="1"/>
         <v>-3.9590110100806722E-2</v>
       </c>
@@ -2539,7 +2544,7 @@
         <f t="shared" si="3"/>
         <v>-961673.78000010177</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23" s="4">
         <f t="shared" si="4"/>
         <v>-4.2394738976719144E-2</v>
       </c>
@@ -2557,7 +2562,7 @@
         <f t="shared" si="6"/>
         <v>-601242.55999999866</v>
       </c>
-      <c r="O23" s="5">
+      <c r="O23" s="4">
         <f t="shared" si="7"/>
         <v>-2.6581238479758625E-2</v>
       </c>
@@ -2580,7 +2585,7 @@
         <f t="shared" si="0"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <f t="shared" si="1"/>
         <v>-1.3334943305713101E-2</v>
       </c>
@@ -2598,7 +2603,7 @@
         <f t="shared" si="3"/>
         <v>-45485.580000000075</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24" s="4">
         <f t="shared" si="4"/>
         <v>-4.087856565111897E-2</v>
       </c>
@@ -2616,7 +2621,7 @@
         <f t="shared" si="6"/>
         <v>-72.879999999888241</v>
       </c>
-      <c r="O24" s="5">
+      <c r="O24" s="4">
         <f t="shared" si="7"/>
         <v>-6.5508515423775231E-5</v>
       </c>
@@ -2639,7 +2644,7 @@
         <f t="shared" si="0"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <f t="shared" si="1"/>
         <v>-1.0226130964676661E-2</v>
       </c>
@@ -2657,7 +2662,7 @@
         <f t="shared" si="3"/>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="4">
         <f t="shared" si="4"/>
         <v>-1.5846773555029746E-2</v>
       </c>
@@ -2675,7 +2680,7 @@
         <f t="shared" si="6"/>
         <v>-1724.9000000000233</v>
       </c>
-      <c r="O25" s="5">
+      <c r="O25" s="4">
         <f t="shared" si="7"/>
         <v>-3.4862304105441511E-3</v>
       </c>
@@ -2698,7 +2703,7 @@
         <f t="shared" si="0"/>
         <v>-447839.91999999993</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <f t="shared" si="1"/>
         <v>-8.5306091660634673E-2</v>
       </c>
@@ -2716,7 +2721,7 @@
         <f t="shared" si="3"/>
         <v>-319870.97000000998</v>
       </c>
-      <c r="J26" s="5">
+      <c r="J26" s="4">
         <f t="shared" si="4"/>
         <v>-5.8776040939327839E-2</v>
       </c>
@@ -2734,7 +2739,7 @@
         <f t="shared" si="6"/>
         <v>-313464.79000000004</v>
       </c>
-      <c r="O26" s="5">
+      <c r="O26" s="4">
         <f t="shared" si="7"/>
         <v>-6.1256670279183835E-2</v>
       </c>
@@ -2757,7 +2762,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2775,7 +2780,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J27" s="5">
+      <c r="J27" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2793,7 +2798,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O27" s="5">
+      <c r="O27" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2816,7 +2821,7 @@
         <f t="shared" si="0"/>
         <v>-132457.97999999998</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="4">
         <f t="shared" si="1"/>
         <v>-9.5782760864849215E-2</v>
       </c>
@@ -2834,7 +2839,7 @@
         <f t="shared" si="3"/>
         <v>-264364.77</v>
       </c>
-      <c r="J28" s="5">
+      <c r="J28" s="4">
         <f t="shared" si="4"/>
         <v>-0.17103239309050916</v>
       </c>
@@ -2852,7 +2857,7 @@
         <f t="shared" si="6"/>
         <v>-132614.93999999994</v>
       </c>
-      <c r="O28" s="5">
+      <c r="O28" s="4">
         <f t="shared" si="7"/>
         <v>-9.5181484254198451E-2</v>
       </c>
@@ -2875,7 +2880,7 @@
         <f t="shared" si="0"/>
         <v>-37915.290000000037</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="4">
         <f t="shared" si="1"/>
         <v>-1.4800253727847622E-2</v>
       </c>
@@ -2893,7 +2898,7 @@
         <f t="shared" si="3"/>
         <v>-114235.56000000983</v>
       </c>
-      <c r="J29" s="5">
+      <c r="J29" s="4">
         <f t="shared" si="4"/>
         <v>-4.1099320021590155E-2</v>
       </c>
@@ -2911,7 +2916,7 @@
         <f t="shared" si="6"/>
         <v>-35.330000000074506</v>
       </c>
-      <c r="O29" s="5">
+      <c r="O29" s="4">
         <f t="shared" si="7"/>
         <v>-1.2225485977540432E-5</v>
       </c>
@@ -2934,7 +2939,7 @@
         <f t="shared" si="0"/>
         <v>-101705.90000000037</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="4">
         <f t="shared" si="1"/>
         <v>-8.3831374359143746E-3</v>
       </c>
@@ -2952,7 +2957,7 @@
         <f t="shared" si="3"/>
         <v>-50385.720000099391</v>
       </c>
-      <c r="J30" s="5">
+      <c r="J30" s="4">
         <f t="shared" si="4"/>
         <v>-3.9561962641116366E-3</v>
       </c>
@@ -2970,7 +2975,7 @@
         <f t="shared" si="6"/>
         <v>-35290.390000000596</v>
       </c>
-      <c r="O30" s="5">
+      <c r="O30" s="4">
         <f t="shared" si="7"/>
         <v>-2.7514707280809998E-3</v>
       </c>
@@ -2993,7 +2998,7 @@
         <f t="shared" si="0"/>
         <v>-24772.310000000056</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="4">
         <f t="shared" si="1"/>
         <v>-1.4030533529678329E-2</v>
       </c>
@@ -3011,7 +3016,7 @@
         <f t="shared" si="3"/>
         <v>-60623.149999999907</v>
       </c>
-      <c r="J31" s="5">
+      <c r="J31" s="4">
         <f t="shared" si="4"/>
         <v>-3.3249136181648611E-2</v>
       </c>
@@ -3029,7 +3034,7 @@
         <f t="shared" si="6"/>
         <v>-69308.659999999916</v>
       </c>
-      <c r="O31" s="5">
+      <c r="O31" s="4">
         <f t="shared" si="7"/>
         <v>-3.847507116360397E-2</v>
       </c>
@@ -3052,7 +3057,7 @@
         <f t="shared" si="0"/>
         <v>-73762.280000009574</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="4">
         <f t="shared" si="1"/>
         <v>-1.2294942827617691E-2</v>
       </c>
@@ -3070,7 +3075,7 @@
         <f t="shared" si="3"/>
         <v>-110514.53000000026</v>
       </c>
-      <c r="J32" s="5">
+      <c r="J32" s="4">
         <f t="shared" si="4"/>
         <v>-1.7837871035428981E-2</v>
       </c>
@@ -3088,7 +3093,7 @@
         <f t="shared" si="6"/>
         <v>-169827.98000000045</v>
       </c>
-      <c r="O32" s="5">
+      <c r="O32" s="4">
         <f t="shared" si="7"/>
         <v>-2.8363413322250185E-2</v>
       </c>
@@ -3111,7 +3116,7 @@
         <f t="shared" si="0"/>
         <v>-7418835.2699990273</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="4">
         <f t="shared" si="1"/>
         <v>-7.9969930789269058E-3</v>
       </c>
@@ -3129,7 +3134,7 @@
         <f t="shared" si="3"/>
         <v>-2602486.5199999809</v>
       </c>
-      <c r="J33" s="5">
+      <c r="J33" s="4">
         <f t="shared" si="4"/>
         <v>-2.6564903115433454E-3</v>
       </c>
@@ -3147,7 +3152,7 @@
         <f t="shared" si="6"/>
         <v>-5456610.5900000334</v>
       </c>
-      <c r="O33" s="5">
+      <c r="O33" s="4">
         <f t="shared" si="7"/>
         <v>-5.5446806934487392E-3</v>
       </c>
@@ -3170,7 +3175,7 @@
         <f t="shared" si="0"/>
         <v>-79341.779999999795</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="4">
         <f t="shared" si="1"/>
         <v>-1.8939149738619768E-2</v>
       </c>
@@ -3188,7 +3193,7 @@
         <f t="shared" si="3"/>
         <v>-213011.23000001023</v>
       </c>
-      <c r="J34" s="5">
+      <c r="J34" s="4">
         <f t="shared" si="4"/>
         <v>-4.8961345561534093E-2</v>
       </c>
@@ -3206,7 +3211,7 @@
         <f t="shared" si="6"/>
         <v>-115798.49000000022</v>
       </c>
-      <c r="O34" s="5">
+      <c r="O34" s="4">
         <f t="shared" si="7"/>
         <v>-2.7376814190035178E-2</v>
       </c>
@@ -3229,7 +3234,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3247,7 +3252,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J35" s="5">
+      <c r="J35" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3265,7 +3270,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O35" s="5">
+      <c r="O35" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3288,7 +3293,7 @@
         <f t="shared" si="0"/>
         <v>-62776.72000000102</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="4">
         <f t="shared" si="1"/>
         <v>-7.8647857679780775E-2</v>
       </c>
@@ -3306,7 +3311,7 @@
         <f t="shared" si="3"/>
         <v>-157733.05000000098</v>
       </c>
-      <c r="J36" s="5">
+      <c r="J36" s="4">
         <f t="shared" si="4"/>
         <v>-0.17551246244575608</v>
       </c>
@@ -3324,7 +3329,7 @@
         <f t="shared" si="6"/>
         <v>-101084.71000000101</v>
       </c>
-      <c r="O36" s="5">
+      <c r="O36" s="4">
         <f t="shared" si="7"/>
         <v>-0.13006011500365766</v>
       </c>
@@ -3347,7 +3352,7 @@
         <f t="shared" si="0"/>
         <v>-82352.260000010021</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="4">
         <f t="shared" si="1"/>
         <v>-3.9444515758219188E-2</v>
       </c>
@@ -3365,7 +3370,7 @@
         <f t="shared" si="3"/>
         <v>-110256.79000000004</v>
       </c>
-      <c r="J37" s="5">
+      <c r="J37" s="4">
         <f t="shared" si="4"/>
         <v>-4.9460250314014013E-2</v>
       </c>
@@ -3383,7 +3388,7 @@
         <f t="shared" si="6"/>
         <v>-188181.66000000015</v>
       </c>
-      <c r="O37" s="5">
+      <c r="O37" s="4">
         <f t="shared" si="7"/>
         <v>-8.9239827069555508E-2</v>
       </c>
@@ -3406,7 +3411,7 @@
         <f t="shared" si="0"/>
         <v>-16630.180000000051</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="4">
         <f t="shared" si="1"/>
         <v>-1.9443680579913542E-2</v>
       </c>
@@ -3424,7 +3429,7 @@
         <f t="shared" si="3"/>
         <v>-39348.040000000037</v>
       </c>
-      <c r="J38" s="5">
+      <c r="J38" s="4">
         <f t="shared" si="4"/>
         <v>-4.9631735620585316E-2</v>
       </c>
@@ -3442,7 +3447,7 @@
         <f t="shared" si="6"/>
         <v>-136.73999999999069</v>
       </c>
-      <c r="O38" s="5">
+      <c r="O38" s="4">
         <f t="shared" si="7"/>
         <v>-1.7583446079218231E-4</v>
       </c>
@@ -3465,7 +3470,7 @@
         <f t="shared" si="0"/>
         <v>-70791.13</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="4">
         <f t="shared" si="1"/>
         <v>-8.008952370177623E-2</v>
       </c>
@@ -3483,7 +3488,7 @@
         <f t="shared" si="3"/>
         <v>-180157.72000000998</v>
       </c>
-      <c r="J39" s="5">
+      <c r="J39" s="4">
         <f t="shared" si="4"/>
         <v>-0.13918241656366656</v>
       </c>
@@ -3501,7 +3506,7 @@
         <f t="shared" si="6"/>
         <v>-79036.1300000099</v>
       </c>
-      <c r="O39" s="5">
+      <c r="O39" s="4">
         <f t="shared" si="7"/>
         <v>-4.7032329234195536E-2</v>
       </c>
@@ -3524,7 +3529,7 @@
         <f t="shared" si="0"/>
         <v>-816758.14000009745</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="4">
         <f t="shared" si="1"/>
         <v>-2.1279773539092578E-2</v>
       </c>
@@ -3542,7 +3547,7 @@
         <f t="shared" si="3"/>
         <v>-1869659.8100000992</v>
       </c>
-      <c r="J40" s="5">
+      <c r="J40" s="4">
         <f t="shared" si="4"/>
         <v>-4.6782546934937892E-2</v>
       </c>
@@ -3560,7 +3565,7 @@
         <f t="shared" si="6"/>
         <v>-610436.29000010341</v>
       </c>
-      <c r="O40" s="5">
+      <c r="O40" s="4">
         <f t="shared" si="7"/>
         <v>-1.5412619944909845E-2</v>
       </c>
@@ -3583,7 +3588,7 @@
         <f t="shared" si="0"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="4">
         <f t="shared" si="1"/>
         <v>-4.0110550149132493E-2</v>
       </c>
@@ -3601,7 +3606,7 @@
         <f t="shared" si="3"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="J41" s="5">
+      <c r="J41" s="4">
         <f t="shared" si="4"/>
         <v>-2.6221894095689226E-2</v>
       </c>
@@ -3619,7 +3624,7 @@
         <f t="shared" si="6"/>
         <v>-82077.349999999627</v>
       </c>
-      <c r="O41" s="5">
+      <c r="O41" s="4">
         <f t="shared" si="7"/>
         <v>-1.7397294491347533E-2</v>
       </c>
@@ -3642,7 +3647,7 @@
         <f t="shared" si="0"/>
         <v>-41624.320001006126</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="4">
         <f t="shared" si="1"/>
         <v>-2.2070943135841053E-4</v>
       </c>
@@ -3660,7 +3665,7 @@
         <f t="shared" si="3"/>
         <v>-2375266.6899999976</v>
       </c>
-      <c r="J42" s="5">
+      <c r="J42" s="4">
         <f t="shared" si="4"/>
         <v>-1.1928203241796942E-2</v>
       </c>
@@ -3678,7 +3683,7 @@
         <f t="shared" si="6"/>
         <v>-36.250001013278961</v>
       </c>
-      <c r="O42" s="5">
+      <c r="O42" s="4">
         <f t="shared" si="7"/>
         <v>-1.8129119102578695E-7</v>
       </c>
@@ -3701,7 +3706,7 @@
         <f t="shared" si="0"/>
         <v>-166754.16999999993</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="4">
         <f t="shared" si="1"/>
         <v>-2.0497353541313264E-2</v>
       </c>
@@ -3719,7 +3724,7 @@
         <f t="shared" si="3"/>
         <v>-389327.98000000045</v>
       </c>
-      <c r="J43" s="5">
+      <c r="J43" s="4">
         <f t="shared" si="4"/>
         <v>-4.5477990374731388E-2</v>
       </c>
@@ -3737,7 +3742,7 @@
         <f t="shared" si="6"/>
         <v>-346517.43000000995</v>
       </c>
-      <c r="O43" s="5">
+      <c r="O43" s="4">
         <f t="shared" si="7"/>
         <v>-4.2512350753316649E-2</v>
       </c>
@@ -3760,7 +3765,7 @@
         <f t="shared" si="0"/>
         <v>-294095.62000000104</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="4">
         <f t="shared" si="1"/>
         <v>-9.7760750186150751E-3</v>
       </c>
@@ -3778,7 +3783,7 @@
         <f t="shared" si="3"/>
         <v>-246988.51999999955</v>
       </c>
-      <c r="J44" s="5">
+      <c r="J44" s="4">
         <f t="shared" si="4"/>
         <v>-7.9569249404813532E-3</v>
       </c>
@@ -3796,7 +3801,7 @@
         <f t="shared" si="6"/>
         <v>-58.75</v>
       </c>
-      <c r="O44" s="5">
+      <c r="O44" s="4">
         <f t="shared" si="7"/>
         <v>-1.8780683691209917E-6</v>
       </c>
@@ -3819,7 +3824,7 @@
         <f t="shared" si="0"/>
         <v>-712015.95000009984</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="4">
         <f t="shared" si="1"/>
         <v>-1.287514194887851E-2</v>
       </c>
@@ -3837,7 +3842,7 @@
         <f t="shared" si="3"/>
         <v>-2197246.0400001034</v>
       </c>
-      <c r="J45" s="5">
+      <c r="J45" s="4">
         <f t="shared" si="4"/>
         <v>-3.8689222111488959E-2</v>
       </c>
@@ -3855,7 +3860,7 @@
         <f t="shared" si="6"/>
         <v>-640550.34000010043</v>
       </c>
-      <c r="O45" s="5">
+      <c r="O45" s="4">
         <f t="shared" si="7"/>
         <v>-1.1565088346037651E-2</v>
       </c>
@@ -3878,7 +3883,7 @@
         <f t="shared" si="0"/>
         <v>-777.57000000000698</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="4">
         <f t="shared" si="1"/>
         <v>-3.0010420686993711E-3</v>
       </c>
@@ -3896,7 +3901,7 @@
         <f t="shared" si="3"/>
         <v>-8597.090000000986</v>
       </c>
-      <c r="J46" s="5">
+      <c r="J46" s="4">
         <f t="shared" si="4"/>
         <v>-3.2319887218048821E-2</v>
       </c>
@@ -3914,7 +3919,7 @@
         <f t="shared" si="6"/>
         <v>-12346.840000000986</v>
       </c>
-      <c r="O46" s="5">
+      <c r="O46" s="4">
         <f t="shared" si="7"/>
         <v>-4.846589537888768E-2</v>
       </c>
@@ -3937,7 +3942,7 @@
         <f t="shared" si="0"/>
         <v>-12273.280000001192</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="4">
         <f t="shared" si="1"/>
         <v>-1.7435939690898361E-4</v>
       </c>
@@ -3955,7 +3960,7 @@
         <f t="shared" si="3"/>
         <v>-24458.340000003576</v>
       </c>
-      <c r="J47" s="5">
+      <c r="J47" s="4">
         <f t="shared" si="4"/>
         <v>-3.3291600310348285E-4</v>
       </c>
@@ -3973,7 +3978,7 @@
         <f t="shared" si="6"/>
         <v>-21970.820000097156</v>
       </c>
-      <c r="O47" s="5">
+      <c r="O47" s="4">
         <f t="shared" si="7"/>
         <v>-2.9274586623690628E-4</v>
       </c>
@@ -3996,7 +4001,7 @@
         <f t="shared" si="0"/>
         <v>-209747.43000000995</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="4">
         <f t="shared" si="1"/>
         <v>-3.1133192323107857E-2</v>
       </c>
@@ -4014,7 +4019,7 @@
         <f t="shared" si="3"/>
         <v>-292627.44000000041</v>
       </c>
-      <c r="J48" s="5">
+      <c r="J48" s="4">
         <f t="shared" si="4"/>
         <v>-4.0559890224125802E-2</v>
       </c>
@@ -4032,7 +4037,7 @@
         <f t="shared" si="6"/>
         <v>-407449.76000001002</v>
       </c>
-      <c r="O48" s="5">
+      <c r="O48" s="4">
         <f t="shared" si="7"/>
         <v>-5.9202125115912531E-2</v>
       </c>
@@ -4055,7 +4060,7 @@
         <f t="shared" si="0"/>
         <v>-1700.570000000007</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="4">
         <f t="shared" si="1"/>
         <v>-1.8444360086767971E-2</v>
       </c>
@@ -4073,7 +4078,7 @@
         <f t="shared" si="3"/>
         <v>-7133.1199999999953</v>
       </c>
-      <c r="J49" s="5">
+      <c r="J49" s="4">
         <f t="shared" si="4"/>
         <v>-6.9523586744639335E-2</v>
       </c>
@@ -4091,7 +4096,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O49" s="5">
+      <c r="O49" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4114,7 +4119,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4132,7 +4137,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J50" s="5">
+      <c r="J50" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4150,7 +4155,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O50" s="5">
+      <c r="O50" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4173,7 +4178,7 @@
         <f t="shared" si="0"/>
         <v>-110074.66000000946</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="4">
         <f t="shared" si="1"/>
         <v>-1.2785255822058129E-2</v>
       </c>
@@ -4191,7 +4196,7 @@
         <f t="shared" si="3"/>
         <v>-326440.38000000082</v>
       </c>
-      <c r="J51" s="5">
+      <c r="J51" s="4">
         <f t="shared" si="4"/>
         <v>-3.6573903982970231E-2</v>
       </c>
@@ -4209,7 +4214,7 @@
         <f t="shared" si="6"/>
         <v>-98056.689999999478</v>
       </c>
-      <c r="O51" s="5">
+      <c r="O51" s="4">
         <f t="shared" si="7"/>
         <v>-1.1224639284424102E-2</v>
       </c>
@@ -4232,7 +4237,7 @@
         <f t="shared" si="0"/>
         <v>-196315.20000000019</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="4">
         <f t="shared" si="1"/>
         <v>-8.009596083231342E-2</v>
       </c>
@@ -4250,7 +4255,7 @@
         <f t="shared" si="3"/>
         <v>-236027.12000000011</v>
       </c>
-      <c r="J52" s="5">
+      <c r="J52" s="4">
         <f t="shared" si="4"/>
         <v>-9.6704683082722218E-2</v>
       </c>
@@ -4268,7 +4273,7 @@
         <f t="shared" si="6"/>
         <v>-264764.74</v>
       </c>
-      <c r="O52" s="5">
+      <c r="O52" s="4">
         <f t="shared" si="7"/>
         <v>-0.12872432962861594</v>
       </c>
@@ -4399,7 +4404,7 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4417,7 +4422,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -4434,7 +4439,7 @@
         <v>-9181.0800000000163</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -4451,7 +4456,7 @@
         <v>-311228.08999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>32</v>
       </c>
@@ -4468,7 +4473,7 @@
         <v>-374962.91000000015</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -4485,7 +4490,7 @@
         <v>-72.879999999888241</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -4502,7 +4507,7 @@
         <v>-1724.9000000000233</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -4519,12 +4524,12 @@
         <v>-82077.349999999627</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" s="7" t="s">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -4538,7 +4543,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -4555,7 +4560,7 @@
         <v>-9181.0800000000163</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -4571,8 +4576,11 @@
         <f t="shared" si="11"/>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H75" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>32</v>
       </c>
@@ -4588,8 +4596,11 @@
         <f t="shared" si="11"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -4606,7 +4617,7 @@
         <v>-72.879999999888241</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -4623,7 +4634,7 @@
         <v>-1724.9000000000233</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -4641,7 +4652,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="6" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4665,11 +4676,11 @@
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="5">
         <f>INDEX(B2:B52,MATCH(B82,A2:A52,0))</f>
         <v>356640100</v>
       </c>
-      <c r="C84" s="6">
+      <c r="C84" s="5">
         <f>INDEX(C2:C52,MATCH(B82,A2:A52))</f>
         <v>341243679.13</v>
       </c>
@@ -4678,11 +4689,11 @@
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="5">
         <f>INDEX(G2:G52,MATCH(B82,A2:A52,0))</f>
         <v>382685200</v>
       </c>
-      <c r="C85" s="6">
+      <c r="C85" s="5">
         <f>INDEX(H2:H52,MATCH(B82,A2:A52,0))</f>
         <v>346340810.81999999</v>
       </c>
@@ -4691,17 +4702,17 @@
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="5">
         <f>INDEX(L2:L52,MATCH(B82,A2:A52,0))</f>
         <v>376548600</v>
       </c>
-      <c r="C86" s="6">
+      <c r="C86" s="5">
         <f>INDEX(M2:M52,MATCH(B82,A2:A52,0))</f>
         <v>355279492.22999901</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4709,35 +4720,35 @@
       <c r="A89" t="s">
         <v>77</v>
       </c>
-      <c r="B89" s="7">
+      <c r="B89" s="6">
         <v>1</v>
       </c>
-      <c r="C89" s="7"/>
-      <c r="D89" s="7">
+      <c r="C89" s="6"/>
+      <c r="D89" s="6">
         <v>2</v>
       </c>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7">
+      <c r="E89" s="6"/>
+      <c r="F89" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B90" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C90" s="8" t="s">
+      <c r="B90" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="8" t="s">
+      <c r="D90" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F90" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G90" s="8" t="s">
+      <c r="F90" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G90" s="7" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4746,27 +4757,27 @@
         <v>73</v>
       </c>
       <c r="B91" t="str">
-        <f>_xlfn.XLOOKUP(B$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <f t="shared" ref="B91:G91" si="12">_xlfn.XLOOKUP(B$89, $F$2:$F$52, $A$2:$A$52)</f>
         <v>Clerk and Master - Chancery</v>
       </c>
-      <c r="C91" s="5">
-        <f>_xlfn.XLOOKUP(B$91, $A$2:$A$52,$E$2:$E$52)</f>
+      <c r="C91" s="4">
+        <f>_xlfn.XLOOKUP(B$89, $F$2:$F$52,$E$2:$E$52)</f>
         <v>-0.15235918433091292</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" ref="C91:G91" si="12">_xlfn.XLOOKUP(D$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <f t="shared" si="12"/>
         <v>Circuit Court Clerk</v>
       </c>
-      <c r="E91" s="5">
-        <f>_xlfn.XLOOKUP(D$91, $A$2:$A$52,$E$2:$E$52)</f>
+      <c r="E91" s="4">
+        <f>_xlfn.XLOOKUP(D$89, $F$2:$F$52,$E$2:$E$52)</f>
         <v>-0.11502817362571344</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="12"/>
         <v>Internal Audit</v>
       </c>
-      <c r="G91" s="5">
-        <f>_xlfn.XLOOKUP(F$91, $A$2:$A$52,$E$2:$E$52)</f>
+      <c r="G91" s="4">
+        <f>_xlfn.XLOOKUP(F$89, $F$2:$F$52,$E$2:$E$52)</f>
         <v>-9.5782760864849215E-2</v>
       </c>
     </row>
@@ -4778,24 +4789,24 @@
         <f>_xlfn.XLOOKUP(B$89, $K$2:$K$52, $A$2:$A$52)</f>
         <v>Metropolitan Clerk</v>
       </c>
-      <c r="C92" s="5">
-        <f>_xlfn.XLOOKUP(B$92, $A$2:$A$52,$J$2:$J$52)</f>
+      <c r="C92" s="4">
+        <f>_xlfn.XLOOKUP(B$89, $K$2:$K$52,$J$2:$J$52)</f>
         <v>-0.17551246244575608</v>
       </c>
       <c r="D92" t="str">
         <f>_xlfn.XLOOKUP(D$89, $K$2:$K$52, $A$2:$A$52)</f>
         <v>Internal Audit</v>
       </c>
-      <c r="E92" s="5">
-        <f>_xlfn.XLOOKUP(D$92, $A$2:$A$52,$J$2:$J$52)</f>
+      <c r="E92" s="4">
+        <f>_xlfn.XLOOKUP(D$89, $K$2:$K$52,$J$2:$J$52)</f>
         <v>-0.17103239309050916</v>
       </c>
       <c r="F92" t="str">
         <f>_xlfn.XLOOKUP(F$89, $K$2:$K$52, $A$2:$A$52)</f>
         <v>Office of Family Safety</v>
       </c>
-      <c r="G92" s="5">
-        <f>_xlfn.XLOOKUP(F$92, $A$2:$A$52,$J$2:$J$52)</f>
+      <c r="G92" s="4">
+        <f>_xlfn.XLOOKUP(F$89, $K$2:$K$52,$J$2:$J$52)</f>
         <v>-0.13918241656366656</v>
       </c>
     </row>
@@ -4807,29 +4818,29 @@
         <f>_xlfn.XLOOKUP(B$89, $P$2:$P$52, $A$2:$A$52)</f>
         <v>Community Oversight Board</v>
       </c>
-      <c r="C93" s="5">
-        <f>_xlfn.XLOOKUP(B$93,$A$2:$A$52,$O$2:$O$52)</f>
+      <c r="C93" s="4">
+        <f>_xlfn.XLOOKUP(B$89,$P$2:$P$52,$O$2:$O$52)</f>
         <v>-4.8803319517950765</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" ref="C93:G93" si="13">_xlfn.XLOOKUP(D$89, $P$2:$P$52, $A$2:$A$52)</f>
         <v>Clerk and Master - Chancery</v>
       </c>
-      <c r="E93" s="5">
-        <f>_xlfn.XLOOKUP(D$93,$A$2:$A$52,$O$2:$O$52)</f>
+      <c r="E93" s="4">
+        <f>_xlfn.XLOOKUP(D$89,$P$2:$P$52,$O$2:$O$52)</f>
         <v>-0.18057733573186341</v>
       </c>
       <c r="F93" t="str">
         <f t="shared" si="13"/>
         <v>Election Commission</v>
       </c>
-      <c r="G93" s="5">
-        <f>_xlfn.XLOOKUP(F$93,$A$2:$A$52,$O$2:$O$52)</f>
+      <c r="G93" s="4">
+        <f>_xlfn.XLOOKUP(F$89,$P$2:$P$52,$O$2:$O$52)</f>
         <v>-0.14787719878320607</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="7" t="s">
+      <c r="A95" s="6" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4837,39 +4848,39 @@
       <c r="A96" t="s">
         <v>77</v>
       </c>
-      <c r="B96" s="7">
+      <c r="B96" s="6">
         <v>1</v>
       </c>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7">
+      <c r="C96" s="6"/>
+      <c r="D96" s="6">
         <v>2</v>
       </c>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7">
+      <c r="E96" s="6"/>
+      <c r="F96" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B97" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C97" s="8" t="s">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D97" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="8" t="s">
+      <c r="D97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F97" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G97" s="8" t="s">
+      <c r="F97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G97" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>73</v>
       </c>
@@ -4877,29 +4888,33 @@
         <f>INDEX($A$2:$A$52,MATCH(B$96,$F$2:$F$52, 0))</f>
         <v>Clerk and Master - Chancery</v>
       </c>
-      <c r="C98" s="5">
-        <f>INDEX($E$2:$E$52,MATCH(B$96,$F$2:$F$52,0))</f>
+      <c r="C98" s="4">
+        <f>INDEX($A$2:$P$52,(MATCH(B98,$A$2:$A$52,0)),MATCH(_xlfn.CONCAT($A98,"??????",$C$90), $A$1:$P$1, 0))</f>
         <v>-0.15235918433091292</v>
       </c>
       <c r="D98" t="str">
         <f>INDEX($A$2:$A$52,MATCH(D$96,$F$2:$F$52, 0))</f>
         <v>Circuit Court Clerk</v>
       </c>
-      <c r="E98" s="5">
-        <f>INDEX($E$2:$E$52, MATCH(D$98, $A$2:$A$52))</f>
+      <c r="E98" s="4">
+        <f>INDEX($A$2:$P$52,(MATCH(D98,$A$2:$A$52,0)),MATCH(_xlfn.CONCAT($A98,"??????",$C$90), $A$1:$P$1, 0))</f>
         <v>-0.11502817362571344</v>
       </c>
       <c r="F98" t="str">
         <f>INDEX($A$2:$A$52,MATCH(F$96,$F$2:$F$52, 0))</f>
         <v>Internal Audit</v>
       </c>
-      <c r="G98" s="5">
-        <f>INDEX($E$2:$E$52, MATCH(F$98, $A$2:$A$52))</f>
+      <c r="G98" s="4">
+        <f>INDEX($A$2:$P$52,(MATCH(F98,$A$2:$A$52,0)),MATCH(_xlfn.CONCAT($A98,"??????",$C$90), $A$1:$P$1, 0))</f>
         <v>-9.5782760864849215E-2</v>
       </c>
-      <c r="I98" s="4"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I98" s="8">
+        <f>INDEX($A$2:$P$52,(MATCH(B98,$A$2:$A$52,0)),MATCH(_xlfn.CONCAT($A98,"??????",$C$90), $A$1:$P$1, 0))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="K98" s="8"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -4907,29 +4922,32 @@
         <f>INDEX($A$2:$A$52,MATCH(B$96,$K$2:$K$52, 0))</f>
         <v>Metropolitan Clerk</v>
       </c>
-      <c r="C99" s="5">
-        <f>INDEX($J$2:$J$52, MATCH(B$99, $A$2:$A$52,0))</f>
+      <c r="C99" s="4">
+        <f t="shared" ref="C99:C100" si="14">INDEX($A$2:$P$52,(MATCH(B99,$A$2:$A$52,0)),MATCH(_xlfn.CONCAT($A99,"??????",$C$90), $A$1:$P$1, 0))</f>
         <v>-0.17551246244575608</v>
       </c>
       <c r="D99" t="str">
         <f>INDEX($A$2:$A$52,MATCH(D$96,$K$2:$K$52, 0))</f>
         <v>Internal Audit</v>
       </c>
-      <c r="E99" s="5">
-        <f>INDEX($J$2:$J$52, MATCH(D$99, $A$2:$A$52,0))</f>
+      <c r="E99" s="4">
+        <f t="shared" ref="E99:E100" si="15">INDEX($A$2:$P$52,(MATCH(D99,$A$2:$A$52,0)),MATCH(_xlfn.CONCAT($A99,"??????",$C$90), $A$1:$P$1, 0))</f>
         <v>-0.17103239309050916</v>
       </c>
       <c r="F99" t="str">
         <f>INDEX($A$2:$A$52,MATCH(F$96,$K$2:$K$52, 0))</f>
         <v>Office of Family Safety</v>
       </c>
-      <c r="G99" s="5">
-        <f>INDEX($J$2:$J$52, MATCH(F$99, $A$2:$A$52,0))</f>
+      <c r="G99" s="4">
+        <f t="shared" ref="G99:G100" si="16">INDEX($A$2:$P$52,(MATCH(F99,$A$2:$A$52,0)),MATCH(_xlfn.CONCAT($A99,"??????",$C$90), $A$1:$P$1, 0))</f>
         <v>-0.13918241656366656</v>
       </c>
-      <c r="I99" s="4"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I99" s="8">
+        <f t="shared" ref="I99:I100" si="17">INDEX($A$2:$P$52,(MATCH(B99,$A$2:$A$52,0)),MATCH(_xlfn.CONCAT($A99,"??????",$C$90), $A$1:$P$1, 0))</f>
+        <v>-0.17551246244575608</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>75</v>
       </c>
@@ -4937,27 +4955,30 @@
         <f>INDEX($A$2:$A$52,MATCH(B$96,$P$2:$P$52,0))</f>
         <v>Community Oversight Board</v>
       </c>
-      <c r="C100" s="5">
-        <f>INDEX($O$2:$O$52, MATCH(B$100, $A$2:$A$52,0))</f>
+      <c r="C100" s="4">
+        <f t="shared" si="14"/>
         <v>-4.8803319517950765</v>
       </c>
       <c r="D100" t="str">
         <f>INDEX($A$2:$A$52,MATCH(D$96,$P$2:$P$52,0))</f>
         <v>Clerk and Master - Chancery</v>
       </c>
-      <c r="E100" s="5">
-        <f>INDEX($O$2:$O$52, MATCH(D$100, $A$2:$A$52,0))</f>
+      <c r="E100" s="4">
+        <f t="shared" si="15"/>
         <v>-0.18057733573186341</v>
       </c>
       <c r="F100" t="str">
         <f>INDEX($A$2:$A$52,MATCH(F$96,$P$2:$P$52,0))</f>
         <v>Election Commission</v>
       </c>
-      <c r="G100" s="5">
-        <f>INDEX($O$2:$O$52, MATCH(F$100, $A$2:$A$52,0))</f>
+      <c r="G100" s="4">
+        <f t="shared" si="16"/>
         <v>-0.14787719878320607</v>
       </c>
-      <c r="I100" s="4"/>
+      <c r="I100" s="8">
+        <f t="shared" si="17"/>
+        <v>-4.8803319517950765</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>